<commit_message>
Fix end to end test following rebase
</commit_message>
<xml_diff>
--- a/gptables/test/expected_workbook.xlsx
+++ b/gptables/test/expected_workbook.xlsx
@@ -123,12 +123,12 @@
     <t>Tests</t>
   </si>
   <si>
-    <t>columnA 
+    <t>columnA
 (Latin alphabet)</t>
   </si>
   <si>
-    <t>columnB 
-(real numbers) 
+    <t>columnB
+(real numbers)
 [note 2]</t>
   </si>
   <si>
@@ -272,8 +272,8 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="table_name" displayName="table_name" ref="A9:B11" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" name="columnA &#10;(Latin alphabet)"/>
-    <tableColumn id="2" name="columnB &#10;(real numbers) &#10;[note 2]"/>
+    <tableColumn id="1" name="columnA&#10;(Latin alphabet)"/>
+    <tableColumn id="2" name="columnB&#10;(real numbers)&#10;[note 2]"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -744,7 +744,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>

<commit_message>
Fix and test columns modifiers (#178)
* Remove trailing whitespace after column header with units added

* Add units placement test

* Remove trailing whitespace after column header with note references added

* Remove NoneType validation exception for units text

* Add table notes placement test

* Fix header modification when units and notes are both added using column name

* Add test for both units and table notes and refactor individual tests

* Add test for additional formatting with units

* Fix integration of table_notes and additional_formatting

* Add tests for additional formatting with table notes

* Update changelog

* Fix end to end test following rebase

* Add comments to clarify column modification checks
</commit_message>
<xml_diff>
--- a/gptables/test/expected_workbook.xlsx
+++ b/gptables/test/expected_workbook.xlsx
@@ -123,12 +123,12 @@
     <t>Tests</t>
   </si>
   <si>
-    <t>columnA 
+    <t>columnA
 (Latin alphabet)</t>
   </si>
   <si>
-    <t>columnB 
-(real numbers) 
+    <t>columnB
+(real numbers)
 [note 2]</t>
   </si>
   <si>
@@ -272,8 +272,8 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="table_name" displayName="table_name" ref="A9:B11" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" name="columnA &#10;(Latin alphabet)"/>
-    <tableColumn id="2" name="columnB &#10;(real numbers) &#10;[note 2]"/>
+    <tableColumn id="1" name="columnA&#10;(Latin alphabet)"/>
+    <tableColumn id="2" name="columnB&#10;(real numbers)&#10;[note 2]"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -744,7 +744,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>

<commit_message>
Added cover page column width customisation and text wrapping (#215)
Co-authored-by: rowanhemsi <rowan.hemsi@ons.gov.uk>
</commit_message>
<xml_diff>
--- a/gptables/test/expected_workbook.xlsx
+++ b/gptables/test/expected_workbook.xlsx
@@ -220,12 +220,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -569,6 +579,9 @@
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="85.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
@@ -631,28 +644,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -681,45 +694,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="7">
+      <c r="A4" s="9">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="7">
+      <c r="A5" s="9">
         <v>2</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="8" t="s">
         <v>21</v>
       </c>
     </row>
@@ -748,66 +761,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="9">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ignore shorthand in _apply_column_alignments
</commit_message>
<xml_diff>
--- a/gptables/test/expected_workbook.xlsx
+++ b/gptables/test/expected_workbook.xlsx
@@ -220,24 +220,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -791,23 +797,23 @@
       <c r="A9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="11">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update end to end test
</commit_message>
<xml_diff>
--- a/gptables/test/expected_workbook.xlsx
+++ b/gptables/test/expected_workbook.xlsx
@@ -153,20 +153,17 @@
     <font>
       <b/>
       <sz val="16"/>
-      <color rgb="FFAUTOMATIC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
-      <color rgb="FFAUTOMATIC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFAUTOMATIC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -180,13 +177,11 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FFAUTOMATIC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FFAUTOMATIC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>

</xml_diff>

<commit_message>
157 automatic colour (#223)
* Update xlsxwriter version

* Update end to end test
</commit_message>
<xml_diff>
--- a/gptables/test/expected_workbook.xlsx
+++ b/gptables/test/expected_workbook.xlsx
@@ -153,20 +153,17 @@
     <font>
       <b/>
       <sz val="16"/>
-      <color rgb="FFAUTOMATIC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
-      <color rgb="FFAUTOMATIC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFAUTOMATIC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -180,13 +177,11 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FFAUTOMATIC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FFAUTOMATIC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>

</xml_diff>

<commit_message>
Update end to end test expected data
</commit_message>
<xml_diff>
--- a/gptables/test/expected_workbook.xlsx
+++ b/gptables/test/expected_workbook.xlsx
@@ -215,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -232,17 +232,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -799,23 +805,23 @@
       <c r="A9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="13">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix alignment for python 3.7
</commit_message>
<xml_diff>
--- a/gptables/test/expected_workbook.xlsx
+++ b/gptables/test/expected_workbook.xlsx
@@ -153,17 +153,20 @@
     <font>
       <b/>
       <sz val="16"/>
+      <color rgb="FFAUTOMATIC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
+      <color rgb="FFAUTOMATIC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FFAUTOMATIC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -177,11 +180,13 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color rgb="FFAUTOMATIC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
+      <color rgb="FFAUTOMATIC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>

</xml_diff>

<commit_message>
Update expected workbook to not contain automatic color
</commit_message>
<xml_diff>
--- a/gptables/test/expected_workbook.xlsx
+++ b/gptables/test/expected_workbook.xlsx
@@ -153,20 +153,17 @@
     <font>
       <b/>
       <sz val="16"/>
-      <color rgb="FFAUTOMATIC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
-      <color rgb="FFAUTOMATIC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFAUTOMATIC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -180,13 +177,11 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FFAUTOMATIC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FFAUTOMATIC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>

</xml_diff>

<commit_message>
213 column alignment (#216)
* Fix include_names parameter in additional_formatting

* Fix unit tests

* Add column alignment based on data type

* WIP: Add more data type options to apply_column_alignments

* Ignore shorthand in _apply_column_alignments

* Add left alignment for index columns

* Update end to end test expected data

* Fix alignment for python 3.7

* Update expected workbook to not contain automatic color

* Add comment to explain use of np.nan instead of None

---------

Co-authored-by: ldavies99 <Luke.Davies@ext.ons.gov.uk>
</commit_message>
<xml_diff>
--- a/gptables/test/expected_workbook.xlsx
+++ b/gptables/test/expected_workbook.xlsx
@@ -215,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -232,17 +232,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -799,23 +805,23 @@
       <c r="A9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="13">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Apply suggested changes and add gridlines to expected workbook in test api
</commit_message>
<xml_diff>
--- a/gptables/test/expected_workbook.xlsx
+++ b/gptables/test/expected_workbook.xlsx
@@ -636,7 +636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -685,7 +685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -753,7 +753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>

<commit_message>
222 gridlines on selected sheets (#228)
* Add gridlines to all sheets except cover

* Add options for user to show or hide gridlines

* Make gridlines off by default

* Apply suggested changes and add gridlines to expected workbook in test api

* Fix numbering on gridlines

* Update expected workbook
</commit_message>
<xml_diff>
--- a/gptables/test/expected_workbook.xlsx
+++ b/gptables/test/expected_workbook.xlsx
@@ -636,7 +636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -674,6 +674,7 @@
   <hyperlinks>
     <hyperlink ref="A4" location="'Label'!A1" display="Label"/>
   </hyperlinks>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -685,7 +686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -742,6 +743,7 @@
     <hyperlink ref="C4" r:id="rId1"/>
     <hyperlink ref="C5" r:id="rId2"/>
   </hyperlinks>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
@@ -753,7 +755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -826,6 +828,7 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>